<commit_message>
Planilha de tarefas atualizada
</commit_message>
<xml_diff>
--- a/Planilha_organização_tarefas_ZERONE.xlsx
+++ b/Planilha_organização_tarefas_ZERONE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27605"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B186AB2D-D323-44FB-8A02-285C7067FF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70AC02EF-35B5-43C5-9DBA-4D1DCEE4D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TASK 07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan </t>
   </si>
   <si>
     <t>Ketlyn</t>
@@ -2571,7 +2568,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B40" sqref="B40:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2872,7 +2869,9 @@
         <v>15</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
       <c r="A21" s="18"/>
@@ -2940,18 +2939,16 @@
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="11"/>
-      <c r="H27" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
       <c r="A28" s="18"/>
@@ -2986,16 +2983,14 @@
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G31" s="11"/>
-      <c r="H31" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
       <c r="A32" s="18"/>
@@ -3023,17 +3018,13 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
       <c r="A35" s="13"/>
-      <c r="B35" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B35" s="9"/>
       <c r="D35" s="13"/>
       <c r="E35" s="9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
       <c r="A36" s="20"/>
@@ -3042,24 +3033,22 @@
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G36" s="20"/>
-      <c r="H36" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="20"/>
       <c r="B37" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37" s="20"/>
-      <c r="E37" s="9"/>
+      <c r="E37" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G37" s="20"/>
-      <c r="H37" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="20"/>
@@ -3084,16 +3073,14 @@
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
       <c r="A40" s="11"/>
       <c r="B40" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G40" s="11"/>
-      <c r="H40" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
       <c r="A41" s="18"/>
@@ -8021,15 +8008,15 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="17"/>
       <c r="D5" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="17"/>
       <c r="G5" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="17"/>
     </row>
@@ -8286,15 +8273,15 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="17"/>
       <c r="D25" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="17"/>
       <c r="G25" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H25" s="17"/>
     </row>
@@ -8479,11 +8466,11 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
       <c r="A45" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" s="17"/>
       <c r="D45" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" s="17"/>
       <c r="H45" s="4"/>

</xml_diff>

<commit_message>
Planilha de tarefas atualizada task6
</commit_message>
<xml_diff>
--- a/Planilha_organização_tarefas_ZERONE.xlsx
+++ b/Planilha_organização_tarefas_ZERONE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27605"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70AC02EF-35B5-43C5-9DBA-4D1DCEE4D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB595C0C-7DB2-47D4-A222-914DB47DCB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -70,6 +70,9 @@
     <t>Erick</t>
   </si>
   <si>
+    <t>Valdeniza</t>
+  </si>
+  <si>
     <t>Alexia</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
   </si>
   <si>
     <t>Vinicius</t>
-  </si>
-  <si>
-    <t>Valdeniza</t>
   </si>
   <si>
     <t>TASK 05</t>
@@ -2567,8 +2567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2669,7 +2669,9 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -2778,10 +2780,12 @@
       <c r="B11" s="12"/>
       <c r="D11" s="11"/>
       <c r="E11" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
       <c r="A12" s="18"/>
@@ -2810,11 +2814,11 @@
     <row r="15" spans="1:26">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="9"/>
@@ -2822,29 +2826,33 @@
     <row r="16" spans="1:26">
       <c r="A16" s="20"/>
       <c r="B16" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="20"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="20"/>
       <c r="B17" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="9"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="20"/>
       <c r="B18" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="9"/>
@@ -2854,7 +2862,7 @@
     <row r="19" spans="1:8">
       <c r="A19" s="21"/>
       <c r="B19" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="10"/>
@@ -2866,11 +2874,11 @@
       <c r="B20" s="12"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
@@ -2939,12 +2947,12 @@
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="11"/>
@@ -2983,11 +2991,11 @@
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="12"/>
@@ -3021,7 +3029,7 @@
       <c r="B35" s="9"/>
       <c r="D35" s="13"/>
       <c r="E35" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="9"/>
@@ -3041,7 +3049,7 @@
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="20"/>
       <c r="B37" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="9" t="s">
@@ -3053,7 +3061,7 @@
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="20"/>
       <c r="B38" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="9"/>
@@ -3063,7 +3071,7 @@
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
       <c r="A39" s="21"/>
       <c r="B39" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="10"/>
@@ -3073,11 +3081,11 @@
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
       <c r="A40" s="11"/>
       <c r="B40" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="12"/>
@@ -8187,7 +8195,7 @@
     <row r="15" spans="1:26">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="9"/>
@@ -8197,7 +8205,7 @@
     <row r="16" spans="1:26">
       <c r="A16" s="20"/>
       <c r="B16" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="9"/>
@@ -8207,7 +8215,7 @@
     <row r="17" spans="1:8">
       <c r="A17" s="20"/>
       <c r="B17" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="9"/>
@@ -8217,7 +8225,7 @@
     <row r="18" spans="1:8">
       <c r="A18" s="20"/>
       <c r="B18" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="9"/>
@@ -8227,7 +8235,7 @@
     <row r="19" spans="1:8">
       <c r="A19" s="21"/>
       <c r="B19" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="10"/>
@@ -8380,7 +8388,7 @@
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
       <c r="A35" s="13"/>
       <c r="B35" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="9"/>
@@ -8390,7 +8398,7 @@
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
       <c r="A36" s="20"/>
       <c r="B36" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="9"/>
@@ -8400,7 +8408,7 @@
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="20"/>
       <c r="B37" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="9"/>
@@ -8410,7 +8418,7 @@
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="20"/>
       <c r="B38" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="9"/>
@@ -8420,7 +8428,7 @@
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
       <c r="A39" s="21"/>
       <c r="B39" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="10"/>
@@ -8553,7 +8561,7 @@
     <row r="55" spans="1:8" ht="15.75" customHeight="1">
       <c r="A55" s="13"/>
       <c r="B55" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="9"/>
@@ -8562,7 +8570,7 @@
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
       <c r="A56" s="20"/>
       <c r="B56" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="9"/>
@@ -8571,7 +8579,7 @@
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
       <c r="A57" s="20"/>
       <c r="B57" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="9"/>
@@ -8580,7 +8588,7 @@
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
       <c r="A58" s="20"/>
       <c r="B58" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="9"/>
@@ -8589,7 +8597,7 @@
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
       <c r="A59" s="21"/>
       <c r="B59" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="10"/>

</xml_diff>